<commit_message>
:D mapiraw na hahha
</commit_message>
<xml_diff>
--- a/bin/questions/File_Management.xlsx
+++ b/bin/questions/File_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\3rd Year UP FILES SEM 2\CMSC 125 (F)\Projects\OSCreate\OSCreate\src\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE756F2-07F1-4045-A93E-D636168ED596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF718610-E104-4315-995A-F9A51AA36BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Question No.</t>
   </si>

</xml_diff>